<commit_message>
Pooh Points: normal 20260201
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-01.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-01.xlsx
@@ -434,7 +434,7 @@
     <col width="26" customWidth="1" min="4" max="4"/>
     <col width="6" customWidth="1" min="5" max="5"/>
     <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="34" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
     <col width="6" customWidth="1" min="8" max="8"/>
     <col width="5" customWidth="1" min="9" max="9"/>
     <col width="5" customWidth="1" min="10" max="10"/>
@@ -1499,20 +1499,20 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I13" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J13" t="n">
         <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
@@ -1521,25 +1521,25 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O13" t="n">
         <v>2</v>
       </c>
       <c r="P13" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="Q13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R13" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="S13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T13" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -2319,47 +2319,47 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="I23" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K23" t="n">
         <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" t="n">
         <v>1</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" t="n">
         <v>2</v>
       </c>
       <c r="P23" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="Q23" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="R23" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="S23" t="n">
         <v>2</v>
       </c>
       <c r="T23" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U23" t="n">
         <v>1</v>
@@ -2401,17 +2401,17 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" t="n">
         <v>0</v>
@@ -2429,13 +2429,13 @@
         <v>0</v>
       </c>
       <c r="P24" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" t="n">
         <v>0</v>
@@ -3057,20 +3057,20 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="I32" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="J32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L32" t="n">
         <v>0</v>
@@ -3079,31 +3079,31 @@
         <v>0</v>
       </c>
       <c r="N32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O32" t="n">
         <v>0</v>
       </c>
       <c r="P32" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="Q32" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R32" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="S32" t="n">
         <v>3</v>
       </c>
       <c r="T32" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V32" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -3139,7 +3139,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H33" t="n">
@@ -3959,53 +3959,53 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="I43" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J43" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K43" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M43" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N43" t="n">
         <v>0</v>
       </c>
       <c r="O43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P43" t="n">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="Q43" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R43" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="S43" t="n">
         <v>0</v>
       </c>
       <c r="T43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V43" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
@@ -4041,47 +4041,47 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H44" t="n">
+        <v>18</v>
+      </c>
+      <c r="I44" t="n">
+        <v>10</v>
+      </c>
+      <c r="J44" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" t="n">
+        <v>7</v>
+      </c>
+      <c r="L44" t="n">
+        <v>6</v>
+      </c>
+      <c r="M44" t="n">
+        <v>0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>0</v>
+      </c>
+      <c r="O44" t="n">
+        <v>2</v>
+      </c>
+      <c r="P44" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>5</v>
+      </c>
+      <c r="R44" t="n">
         <v>11</v>
       </c>
-      <c r="I44" t="n">
-        <v>8</v>
-      </c>
-      <c r="J44" t="n">
-        <v>1</v>
-      </c>
-      <c r="K44" t="n">
-        <v>4</v>
-      </c>
-      <c r="L44" t="n">
-        <v>3</v>
-      </c>
-      <c r="M44" t="n">
-        <v>0</v>
-      </c>
-      <c r="N44" t="n">
-        <v>0</v>
-      </c>
-      <c r="O44" t="n">
-        <v>1</v>
-      </c>
-      <c r="P44" t="n">
-        <v>18</v>
-      </c>
-      <c r="Q44" t="n">
-        <v>4</v>
-      </c>
-      <c r="R44" t="n">
-        <v>9</v>
-      </c>
       <c r="S44" t="n">
         <v>0</v>
       </c>
       <c r="T44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U44" t="n">
         <v>0</v>
@@ -4123,17 +4123,17 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>-4</v>
+        <v>1</v>
       </c>
       <c r="I45" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K45" t="n">
         <v>0</v>
@@ -4151,19 +4151,19 @@
         <v>1</v>
       </c>
       <c r="P45" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="Q45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R45" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S45" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T45" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U45" t="n">
         <v>0</v>
@@ -4943,17 +4943,17 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I55" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J55" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K55" t="n">
         <v>2</v>
@@ -4968,22 +4968,22 @@
         <v>0</v>
       </c>
       <c r="O55" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P55" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="Q55" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R55" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="S55" t="n">
         <v>0</v>
       </c>
       <c r="T55" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U55" t="n">
         <v>0</v>
@@ -5025,47 +5025,47 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I56" t="n">
         <v>2</v>
       </c>
       <c r="J56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L56" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" t="n">
         <v>0</v>
       </c>
       <c r="N56" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O56" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P56" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="Q56" t="n">
         <v>1</v>
       </c>
       <c r="R56" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S56" t="n">
         <v>0</v>
       </c>
       <c r="T56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U56" t="n">
         <v>0</v>
@@ -5763,17 +5763,17 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H65" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I65" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J65" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="K65" t="n">
         <v>2</v>
@@ -5782,22 +5782,22 @@
         <v>1</v>
       </c>
       <c r="M65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N65" t="n">
         <v>0</v>
       </c>
       <c r="O65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P65" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="Q65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R65" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="S65" t="n">
         <v>0</v>
@@ -5806,10 +5806,10 @@
         <v>0</v>
       </c>
       <c r="U65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V65" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
@@ -5845,17 +5845,17 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H66" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I66" t="n">
         <v>5</v>
       </c>
       <c r="J66" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K66" t="n">
         <v>1</v>
@@ -5870,10 +5870,10 @@
         <v>1</v>
       </c>
       <c r="O66" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P66" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Q66" t="n">
         <v>1</v>
@@ -6829,20 +6829,20 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H78" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I78" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J78" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L78" t="n">
         <v>0</v>
@@ -6854,16 +6854,16 @@
         <v>0</v>
       </c>
       <c r="O78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P78" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="Q78" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R78" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S78" t="n">
         <v>0</v>
@@ -12405,17 +12405,17 @@
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H146" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I146" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J146" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K146" t="n">
         <v>0</v>
@@ -12424,22 +12424,22 @@
         <v>0</v>
       </c>
       <c r="M146" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O146" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P146" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="Q146" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R146" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S146" t="n">
         <v>0</v>
@@ -12451,7 +12451,7 @@
         <v>2</v>
       </c>
       <c r="V146" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147">
@@ -12487,20 +12487,20 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H147" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I147" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J147" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K147" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L147" t="n">
         <v>0</v>
@@ -12512,22 +12512,22 @@
         <v>0</v>
       </c>
       <c r="O147" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P147" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="Q147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R147" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S147" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U147" t="n">
         <v>0</v>
@@ -12569,7 +12569,7 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H148" t="n">
@@ -12594,10 +12594,10 @@
         <v>0</v>
       </c>
       <c r="O148" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P148" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q148" t="n">
         <v>1</v>
@@ -12636,7 +12636,7 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Noah Williamson</t>
+          <t>London Jemison</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -12651,17 +12651,17 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I149" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K149" t="n">
         <v>0</v>
@@ -12670,7 +12670,7 @@
         <v>0</v>
       </c>
       <c r="M149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N149" t="n">
         <v>0</v>
@@ -12679,19 +12679,19 @@
         <v>0</v>
       </c>
       <c r="P149" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R149" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T149" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U149" t="n">
         <v>0</v>
@@ -12718,7 +12718,7 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>London Jemison</t>
+          <t>Noah Williamson</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -12733,17 +12733,17 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>Sun, February 1st at 1:00 PM EST</t>
+          <t>18:55 - 2nd Half</t>
         </is>
       </c>
       <c r="H150" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I150" t="n">
         <v>0</v>
       </c>
       <c r="J150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K150" t="n">
         <v>0</v>
@@ -12761,13 +12761,13 @@
         <v>0</v>
       </c>
       <c r="P150" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q150" t="n">
         <v>0</v>
       </c>
       <c r="R150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S150" t="n">
         <v>0</v>
@@ -12830,7 +12830,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -12843,7 +12843,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C3" t="n">
         <v>5</v>
@@ -12856,7 +12856,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C4" t="n">
         <v>5</v>
@@ -12865,27 +12865,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Hilton Heads</t>
+          <t>G-Flop</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>G-Flop</t>
+          <t>Hilton Heads</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -12895,7 +12895,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C7" t="n">
         <v>5</v>

</xml_diff>

<commit_message>
Pooh Points: final 20260201 -> PD9
</commit_message>
<xml_diff>
--- a/docs/Today_PoohPoints_SEC_ByOwner_2026-02-01.xlsx
+++ b/docs/Today_PoohPoints_SEC_ByOwner_2026-02-01.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V151"/>
+  <dimension ref="A1:V156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -1512,7 +1512,7 @@
         <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L13" t="n">
         <v>0</v>
@@ -1527,19 +1527,19 @@
         <v>2</v>
       </c>
       <c r="P13" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="Q13" t="n">
         <v>5</v>
       </c>
       <c r="R13" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="S13" t="n">
         <v>4</v>
       </c>
       <c r="T13" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="U13" t="n">
         <v>0</v>
@@ -2319,17 +2319,17 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I23" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J23" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K23" t="n">
         <v>1</v>
@@ -2347,7 +2347,7 @@
         <v>2</v>
       </c>
       <c r="P23" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="Q23" t="n">
         <v>9</v>
@@ -2362,10 +2362,10 @@
         <v>6</v>
       </c>
       <c r="U23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V23" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -3057,7 +3057,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H32" t="n">
@@ -3124,7 +3124,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Jalil Bethea</t>
+          <t>Taylor Bol Bowen</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -3139,7 +3139,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H33" t="n">
@@ -3164,10 +3164,10 @@
         <v>0</v>
       </c>
       <c r="O33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P33" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q33" t="n">
         <v>0</v>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Taylor Bol Bowen</t>
+          <t>Jalil Bethea</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -3221,17 +3221,17 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" t="n">
         <v>0</v>
@@ -3246,22 +3246,22 @@
         <v>0</v>
       </c>
       <c r="O34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q34" t="n">
         <v>0</v>
       </c>
       <c r="R34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S34" t="n">
         <v>0</v>
       </c>
       <c r="T34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="U34" t="n">
         <v>0</v>
@@ -4041,21 +4041,21 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I44" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="J44" t="n">
+        <v>7</v>
+      </c>
+      <c r="K44" t="n">
         <v>6</v>
       </c>
-      <c r="K44" t="n">
-        <v>5</v>
-      </c>
       <c r="L44" t="n">
         <v>2</v>
       </c>
@@ -4069,13 +4069,13 @@
         <v>2</v>
       </c>
       <c r="P44" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q44" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R44" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="S44" t="n">
         <v>0</v>
@@ -4087,7 +4087,7 @@
         <v>3</v>
       </c>
       <c r="V44" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
@@ -4123,20 +4123,20 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I45" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K45" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L45" t="n">
         <v>8</v>
@@ -4151,7 +4151,7 @@
         <v>2</v>
       </c>
       <c r="P45" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="Q45" t="n">
         <v>6</v>
@@ -4166,10 +4166,10 @@
         <v>1</v>
       </c>
       <c r="U45" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V45" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
@@ -4205,7 +4205,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H46" t="n">
@@ -5010,12 +5010,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Amari Allen</t>
+          <t>Xaivian Lee</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -5025,20 +5025,20 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H56" t="n">
         <v>4</v>
       </c>
       <c r="I56" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J56" t="n">
         <v>3</v>
       </c>
       <c r="K56" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L56" t="n">
         <v>1</v>
@@ -5047,25 +5047,25 @@
         <v>0</v>
       </c>
       <c r="N56" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P56" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R56" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T56" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U56" t="n">
         <v>0</v>
@@ -5092,12 +5092,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Xaivian Lee</t>
+          <t>Amari Allen</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -5107,20 +5107,20 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J57" t="n">
         <v>3</v>
       </c>
       <c r="K57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L57" t="n">
         <v>1</v>
@@ -5129,25 +5129,25 @@
         <v>0</v>
       </c>
       <c r="N57" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O57" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P57" t="n">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="Q57" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R57" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="S57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T57" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U57" t="n">
         <v>0</v>
@@ -5845,17 +5845,17 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H66" t="n">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I66" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J66" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K66" t="n">
         <v>3</v>
@@ -5873,13 +5873,13 @@
         <v>1</v>
       </c>
       <c r="P66" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="Q66" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R66" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S66" t="n">
         <v>0</v>
@@ -5888,10 +5888,10 @@
         <v>0</v>
       </c>
       <c r="U66" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="V66" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
@@ -5927,14 +5927,14 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H67" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I67" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J67" t="n">
         <v>4</v>
@@ -5949,25 +5949,25 @@
         <v>0</v>
       </c>
       <c r="N67" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O67" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P67" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q67" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R67" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S67" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T67" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="U67" t="n">
         <v>2</v>
@@ -6911,11 +6911,11 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H79" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I79" t="n">
         <v>13</v>
@@ -6924,7 +6924,7 @@
         <v>5</v>
       </c>
       <c r="K79" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L79" t="n">
         <v>0</v>
@@ -6939,7 +6939,7 @@
         <v>1</v>
       </c>
       <c r="P79" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q79" t="n">
         <v>5</v>
@@ -12487,20 +12487,20 @@
       </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H147" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I147" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J147" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K147" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L147" t="n">
         <v>0</v>
@@ -12515,7 +12515,7 @@
         <v>4</v>
       </c>
       <c r="P147" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="Q147" t="n">
         <v>4</v>
@@ -12530,10 +12530,10 @@
         <v>2</v>
       </c>
       <c r="U147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V147" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148">
@@ -12569,17 +12569,17 @@
       </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H148" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I148" t="n">
         <v>6</v>
       </c>
       <c r="J148" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K148" t="n">
         <v>0</v>
@@ -12594,10 +12594,10 @@
         <v>2</v>
       </c>
       <c r="O148" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P148" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q148" t="n">
         <v>2</v>
@@ -12636,12 +12636,12 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>Isaiah Brown</t>
+          <t>London Jemison</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>FLA</t>
+          <t>ALA</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -12651,14 +12651,14 @@
       </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H149" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I149" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J149" t="n">
         <v>0</v>
@@ -12670,34 +12670,34 @@
         <v>0</v>
       </c>
       <c r="M149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N149" t="n">
         <v>0</v>
       </c>
       <c r="O149" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P149" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q149" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R149" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S149" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T149" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V149" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -12718,12 +12718,12 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>London Jemison</t>
+          <t>Isaiah Brown</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>ALA</t>
+          <t>FLA</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -12733,7 +12733,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>7:47 - 2nd Half</t>
+          <t>3:36 - 2nd Half</t>
         </is>
       </c>
       <c r="H150" t="n">
@@ -12752,34 +12752,34 @@
         <v>0</v>
       </c>
       <c r="M150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N150" t="n">
         <v>0</v>
       </c>
       <c r="O150" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P150" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q150" t="n">
         <v>1</v>
       </c>
       <c r="R150" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T150" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U150" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V150" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
@@ -12800,67 +12800,477 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
+          <t>Olivier Rioux</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>FLA</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>ALA@FLA</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>3:36 - 2nd Half</t>
+        </is>
+      </c>
+      <c r="H151" t="n">
+        <v>2</v>
+      </c>
+      <c r="I151" t="n">
+        <v>2</v>
+      </c>
+      <c r="J151" t="n">
+        <v>1</v>
+      </c>
+      <c r="K151" t="n">
+        <v>0</v>
+      </c>
+      <c r="L151" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" t="n">
+        <v>0</v>
+      </c>
+      <c r="N151" t="n">
+        <v>0</v>
+      </c>
+      <c r="O151" t="n">
+        <v>0</v>
+      </c>
+      <c r="P151" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q151" t="n">
+        <v>1</v>
+      </c>
+      <c r="R151" t="n">
+        <v>2</v>
+      </c>
+      <c r="S151" t="n">
+        <v>0</v>
+      </c>
+      <c r="T151" t="n">
+        <v>0</v>
+      </c>
+      <c r="U151" t="n">
+        <v>0</v>
+      </c>
+      <c r="V151" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
           <t>Noah Williamson</t>
         </is>
       </c>
-      <c r="E151" t="inlineStr">
+      <c r="E152" t="inlineStr">
         <is>
           <t>ALA</t>
         </is>
       </c>
-      <c r="F151" t="inlineStr">
+      <c r="F152" t="inlineStr">
         <is>
           <t>ALA@FLA</t>
         </is>
       </c>
-      <c r="G151" t="inlineStr">
-        <is>
-          <t>7:47 - 2nd Half</t>
-        </is>
-      </c>
-      <c r="H151" t="n">
-        <v>1</v>
-      </c>
-      <c r="I151" t="n">
-        <v>0</v>
-      </c>
-      <c r="J151" t="n">
-        <v>1</v>
-      </c>
-      <c r="K151" t="n">
-        <v>0</v>
-      </c>
-      <c r="L151" t="n">
-        <v>0</v>
-      </c>
-      <c r="M151" t="n">
-        <v>0</v>
-      </c>
-      <c r="N151" t="n">
-        <v>0</v>
-      </c>
-      <c r="O151" t="n">
-        <v>0</v>
-      </c>
-      <c r="P151" t="n">
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>3:36 - 2nd Half</t>
+        </is>
+      </c>
+      <c r="H152" t="n">
+        <v>1</v>
+      </c>
+      <c r="I152" t="n">
+        <v>0</v>
+      </c>
+      <c r="J152" t="n">
+        <v>1</v>
+      </c>
+      <c r="K152" t="n">
+        <v>0</v>
+      </c>
+      <c r="L152" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" t="n">
+        <v>0</v>
+      </c>
+      <c r="N152" t="n">
+        <v>0</v>
+      </c>
+      <c r="O152" t="n">
+        <v>0</v>
+      </c>
+      <c r="P152" t="n">
         <v>5</v>
       </c>
-      <c r="Q151" t="n">
-        <v>0</v>
-      </c>
-      <c r="R151" t="n">
-        <v>0</v>
-      </c>
-      <c r="S151" t="n">
-        <v>0</v>
-      </c>
-      <c r="T151" t="n">
-        <v>0</v>
-      </c>
-      <c r="U151" t="n">
-        <v>0</v>
-      </c>
-      <c r="V151" t="n">
+      <c r="Q152" t="n">
+        <v>0</v>
+      </c>
+      <c r="R152" t="n">
+        <v>0</v>
+      </c>
+      <c r="S152" t="n">
+        <v>0</v>
+      </c>
+      <c r="T152" t="n">
+        <v>0</v>
+      </c>
+      <c r="U152" t="n">
+        <v>0</v>
+      </c>
+      <c r="V152" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Alex Kovatchev</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>FLA</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>ALA@FLA</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>3:36 - 2nd Half</t>
+        </is>
+      </c>
+      <c r="H153" t="n">
+        <v>0</v>
+      </c>
+      <c r="I153" t="n">
+        <v>0</v>
+      </c>
+      <c r="J153" t="n">
+        <v>0</v>
+      </c>
+      <c r="K153" t="n">
+        <v>0</v>
+      </c>
+      <c r="L153" t="n">
+        <v>0</v>
+      </c>
+      <c r="M153" t="n">
+        <v>0</v>
+      </c>
+      <c r="N153" t="n">
+        <v>0</v>
+      </c>
+      <c r="O153" t="n">
+        <v>0</v>
+      </c>
+      <c r="P153" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q153" t="n">
+        <v>0</v>
+      </c>
+      <c r="R153" t="n">
+        <v>0</v>
+      </c>
+      <c r="S153" t="n">
+        <v>0</v>
+      </c>
+      <c r="T153" t="n">
+        <v>0</v>
+      </c>
+      <c r="U153" t="n">
+        <v>0</v>
+      </c>
+      <c r="V153" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Alex Lloyd</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>FLA</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>ALA@FLA</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>3:36 - 2nd Half</t>
+        </is>
+      </c>
+      <c r="H154" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" t="n">
+        <v>0</v>
+      </c>
+      <c r="J154" t="n">
+        <v>0</v>
+      </c>
+      <c r="K154" t="n">
+        <v>0</v>
+      </c>
+      <c r="L154" t="n">
+        <v>0</v>
+      </c>
+      <c r="M154" t="n">
+        <v>0</v>
+      </c>
+      <c r="N154" t="n">
+        <v>0</v>
+      </c>
+      <c r="O154" t="n">
+        <v>0</v>
+      </c>
+      <c r="P154" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q154" t="n">
+        <v>0</v>
+      </c>
+      <c r="R154" t="n">
+        <v>0</v>
+      </c>
+      <c r="S154" t="n">
+        <v>0</v>
+      </c>
+      <c r="T154" t="n">
+        <v>0</v>
+      </c>
+      <c r="U154" t="n">
+        <v>0</v>
+      </c>
+      <c r="V154" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>CJ Ingram</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>FLA</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>ALA@FLA</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>3:36 - 2nd Half</t>
+        </is>
+      </c>
+      <c r="H155" t="n">
+        <v>0</v>
+      </c>
+      <c r="I155" t="n">
+        <v>0</v>
+      </c>
+      <c r="J155" t="n">
+        <v>0</v>
+      </c>
+      <c r="K155" t="n">
+        <v>0</v>
+      </c>
+      <c r="L155" t="n">
+        <v>0</v>
+      </c>
+      <c r="M155" t="n">
+        <v>0</v>
+      </c>
+      <c r="N155" t="n">
+        <v>0</v>
+      </c>
+      <c r="O155" t="n">
+        <v>0</v>
+      </c>
+      <c r="P155" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q155" t="n">
+        <v>0</v>
+      </c>
+      <c r="R155" t="n">
+        <v>0</v>
+      </c>
+      <c r="S155" t="n">
+        <v>0</v>
+      </c>
+      <c r="T155" t="n">
+        <v>0</v>
+      </c>
+      <c r="U155" t="n">
+        <v>0</v>
+      </c>
+      <c r="V155" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>2026-02-01</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Undrafted</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Viktor Mikic</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>FLA</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>ALA@FLA</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>3:36 - 2nd Half</t>
+        </is>
+      </c>
+      <c r="H156" t="n">
+        <v>0</v>
+      </c>
+      <c r="I156" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" t="n">
+        <v>0</v>
+      </c>
+      <c r="K156" t="n">
+        <v>0</v>
+      </c>
+      <c r="L156" t="n">
+        <v>0</v>
+      </c>
+      <c r="M156" t="n">
+        <v>0</v>
+      </c>
+      <c r="N156" t="n">
+        <v>0</v>
+      </c>
+      <c r="O156" t="n">
+        <v>0</v>
+      </c>
+      <c r="P156" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q156" t="n">
+        <v>0</v>
+      </c>
+      <c r="R156" t="n">
+        <v>0</v>
+      </c>
+      <c r="S156" t="n">
+        <v>0</v>
+      </c>
+      <c r="T156" t="n">
+        <v>0</v>
+      </c>
+      <c r="U156" t="n">
+        <v>0</v>
+      </c>
+      <c r="V156" t="n">
         <v>0</v>
       </c>
     </row>
@@ -12912,7 +13322,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -12925,7 +13335,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" t="n">
         <v>5</v>
@@ -12938,7 +13348,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C4" t="n">
         <v>5</v>
@@ -12951,7 +13361,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C5" t="n">
         <v>5</v>

</xml_diff>